<commit_message>
Add automatically computed results to excel sheet
</commit_message>
<xml_diff>
--- a/kri-evaluation/KRI Liver Segmentation Evaluation v1.xlsx
+++ b/kri-evaluation/KRI Liver Segmentation Evaluation v1.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorgue Guerra\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Master thesis\master\kri-evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E19FE5A-4FD3-4D78-8FC7-8A8E94C970D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FC8D7A-3DC4-41F4-BCB8-75A4C49D7F11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kri" sheetId="1" r:id="rId1"/>
     <sheet name="kriNN" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="etc" sheetId="2" r:id="rId3"/>
+    <sheet name="exported-results" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">kri!$A$1:$F$104</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -216,6 +217,18 @@
   </si>
   <si>
     <t>Multiple volumes are broken, fragmented. Some preprocessing must be done</t>
+  </si>
+  <si>
+    <t>[SIRT]</t>
+  </si>
+  <si>
+    <t>13.05.2020</t>
+  </si>
+  <si>
+    <t>14.05.2020</t>
+  </si>
+  <si>
+    <t>Automatically computed lowdose</t>
   </si>
 </sst>
 </file>
@@ -657,7 +670,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -809,6 +822,27 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -833,26 +867,29 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -946,16 +983,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>305675</xdr:colOff>
+      <xdr:colOff>29450</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>152687</xdr:rowOff>
+      <xdr:rowOff>143162</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -978,7 +1015,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="742950" y="381000"/>
+          <a:off x="466725" y="371475"/>
           <a:ext cx="6268325" cy="2057687"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5543,7 +5580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFB2F4E-B686-4E60-A852-482BEABCB216}">
   <dimension ref="A1:V192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
     </sheetView>
@@ -5715,10 +5752,10 @@
       <c r="P4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="R4" s="63" t="s">
+      <c r="R4" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="63"/>
+      <c r="S4" s="55"/>
       <c r="U4" s="27" t="s">
         <v>2</v>
       </c>
@@ -5770,10 +5807,10 @@
         <f>AVERAGEIFS(G2:G104,G2:G104,"&lt;&gt;0",G2:G104,"&lt;50%")</f>
         <v>5.5461624026696348E-2</v>
       </c>
-      <c r="U5" s="54" t="s">
+      <c r="U5" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="V5" s="51" t="s">
+      <c r="V5" s="58" t="s">
         <v>60</v>
       </c>
     </row>
@@ -5813,8 +5850,8 @@
         <f>STDEV(G2:G104)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U6" s="55"/>
-      <c r="V6" s="52"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="59"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
@@ -5860,8 +5897,8 @@
         <f>AVERAGEIF(H4:H106,"&lt;&gt;0")</f>
         <v>0.89749999999999996</v>
       </c>
-      <c r="U7" s="55"/>
-      <c r="V7" s="52"/>
+      <c r="U7" s="62"/>
+      <c r="V7" s="59"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="24">
@@ -5903,8 +5940,8 @@
       <c r="P8" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="U8" s="55"/>
-      <c r="V8" s="52"/>
+      <c r="U8" s="62"/>
+      <c r="V8" s="59"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
@@ -5943,12 +5980,12 @@
         <f t="shared" si="0"/>
         <v>7.5711987127916255E-2</v>
       </c>
-      <c r="R9" s="63" t="s">
+      <c r="R9" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="S9" s="63"/>
-      <c r="U9" s="57"/>
-      <c r="V9" s="58"/>
+      <c r="S9" s="55"/>
+      <c r="U9" s="64"/>
+      <c r="V9" s="65"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
@@ -5986,10 +6023,10 @@
         <f>AVERAGEIFS(K2:K104,K2:K104,"&lt;&gt;0",K2:K104,"&lt;30%")</f>
         <v>6.3609986190155884E-2</v>
       </c>
-      <c r="U10" s="54" t="s">
+      <c r="U10" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="V10" s="51" t="s">
+      <c r="V10" s="58" t="s">
         <v>58</v>
       </c>
     </row>
@@ -6037,8 +6074,8 @@
         <f>STDEV(K2:K104)</f>
         <v>0.21826631915929956</v>
       </c>
-      <c r="U11" s="55"/>
-      <c r="V11" s="52"/>
+      <c r="U11" s="62"/>
+      <c r="V11" s="59"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="24">
@@ -6084,8 +6121,8 @@
         <f>AVERAGEIF(L4:L106,"&lt;&gt;0")</f>
         <v>0.90393372549019602</v>
       </c>
-      <c r="U12" s="55"/>
-      <c r="V12" s="52"/>
+      <c r="U12" s="62"/>
+      <c r="V12" s="59"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
@@ -6118,8 +6155,8 @@
       </c>
       <c r="R13"/>
       <c r="S13"/>
-      <c r="U13" s="55"/>
-      <c r="V13" s="52"/>
+      <c r="U13" s="62"/>
+      <c r="V13" s="59"/>
     </row>
     <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
@@ -6158,12 +6195,12 @@
         <f t="shared" si="0"/>
         <v>4.6106438980548205E-2</v>
       </c>
-      <c r="R14" s="64" t="s">
+      <c r="R14" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="S14" s="65"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="58"/>
+      <c r="S14" s="57"/>
+      <c r="U14" s="64"/>
+      <c r="V14" s="65"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
@@ -6201,10 +6238,10 @@
         <f>AVERAGEIFS(O2:O104,O2:O104,"&lt;&gt;0",O2:O104,"&lt;50%")</f>
         <v>0.12434032373984207</v>
       </c>
-      <c r="U15" s="54" t="s">
+      <c r="U15" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="V15" s="51" t="s">
+      <c r="V15" s="58" t="s">
         <v>31</v>
       </c>
     </row>
@@ -6244,8 +6281,8 @@
         <f>STDEV(O2:O104)</f>
         <v>0.14978376778042762</v>
       </c>
-      <c r="U16" s="55"/>
-      <c r="V16" s="52"/>
+      <c r="U16" s="62"/>
+      <c r="V16" s="59"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
@@ -6276,8 +6313,8 @@
         <f t="shared" si="0"/>
         <v>4.5371036467268006E-2</v>
       </c>
-      <c r="U17" s="55"/>
-      <c r="V17" s="52"/>
+      <c r="U17" s="62"/>
+      <c r="V17" s="59"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
@@ -6308,8 +6345,8 @@
         <f t="shared" si="0"/>
         <v>0.2329903750414869</v>
       </c>
-      <c r="U18" s="55"/>
-      <c r="V18" s="52"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="59"/>
     </row>
     <row r="19" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24">
@@ -6340,8 +6377,8 @@
         <f t="shared" si="0"/>
         <v>0.26341668729883638</v>
       </c>
-      <c r="U19" s="56"/>
-      <c r="V19" s="53"/>
+      <c r="U19" s="63"/>
+      <c r="V19" s="60"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
@@ -9279,10 +9316,10 @@
       <c r="L106" s="32"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B107" s="59" t="s">
+      <c r="B107" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="C107" s="60"/>
+      <c r="C107" s="52"/>
       <c r="D107" s="47">
         <f>COUNTIF(D2:D104,"=mr")</f>
         <v>55</v>
@@ -9291,10 +9328,10 @@
       <c r="L107" s="32"/>
     </row>
     <row r="108" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="61" t="s">
+      <c r="B108" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="C108" s="62"/>
+      <c r="C108" s="54"/>
       <c r="D108" s="48">
         <f>COUNTIF(D2:D104,"=ct")</f>
         <v>47</v>
@@ -9640,17 +9677,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R14:S14"/>
     <mergeCell ref="V15:V19"/>
     <mergeCell ref="U15:U19"/>
     <mergeCell ref="U5:U9"/>
     <mergeCell ref="V5:V9"/>
     <mergeCell ref="U10:U14"/>
     <mergeCell ref="V10:V14"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R14:S14"/>
   </mergeCells>
   <conditionalFormatting sqref="O2:O104">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
@@ -9677,7 +9714,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9687,59 +9724,1713 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DLCPolicyLabelClientValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">{_UIVersionString}</DLCPolicyLabelClientValue>
-    <_dlc_BarcodeImage xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">iVBORw0KGgoAAAANSUhEUgAAAYIAAABtCAYAAACsn2ZqAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAAAJcEhZcwAADsMAAA7DAcdvqGQAABp9SURBVHhe7ZvBihzbsiz3///0eeiBgeGE54qsTA0uSgMfWLt3aA2aqpH++9/Hx8fHxz/N90Xw8fHx8Y/zfRF8fHx8/ON8XwQfHx8f/zjfF8HHx8fHP873RfDx8fHxj/P6F8F///33/zORHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef/ix8fHx8f/Kb4vgo+Pj49/nO+L4OPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+/irtP7/wH2OmwNQRc9XBWxu46k93snfMVffx8SbfX9fHX+XuB5j3m9+dNvmztzamdb/+W8nmzsfHW3x/WR9/hT8fWmRLbk+/e9XTbTZX5OaPk+Tqnrur3Yknv/vx0fj+qj7+Knc+uHJ7+t2rnm6zuaJtpp9v/63Nv9t48rsfH43vr+rjr7L94Jp2f36WSU4/m3q46v7wy+9OP8+f/fHMljvbj48t31/Vx19l+8H1ZPfnZ46Z9jB17U5yuru9A5vd9tbHx12+v6yPv8rf+IDzfvrd/FnbTD83V33r2r+14Zd/7+PjDb6/ro+/yuYD7O6HHPs7H5x/3OFnJ9pm+vnVvbf/rY+PN/n+wj7+KqcPsV8+5Pidq9/d3H2ymX7+N96z+b2Pj6d8f2Uff5XTB9kvH3T8ztXvvvXvtt308yfv+UNuNr/z8fEG31/ax1/lyYfj1G8+LN+4+4erO63b3Pl18/Hxt/j+2j7+Cn8+yDLJ9LPkdOMPp82ph80uN9Pu1P/htMne+fh4m++v6uPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+Pj4+/nG+L4KPj4+Pf5r//e//AYQWEYJwHQKsAAAAAElFTkSuQmCC</_dlc_BarcodeImage>
-    <DLCPolicyLabelLock xmlns="e2656bbd-0e15-4aa0-af00-25744e385561" xsi:nil="true"/>
-    <_dlc_BarcodeValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">1758931852</_dlc_BarcodeValue>
-    <_dlc_BarcodePreview xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">
-      <Url>https://surgiceye.sharepoint.com/dev/_layouts/15/barcodeimagefromitem.aspx?ID=419111&amp;list=e2656bbd-0e15-4aa0-af00-25744e385561</Url>
-      <Description>Barcode: 1758931852</Description>
-    </_dlc_BarcodePreview>
-    <DLCPolicyLabelValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">0.3</DLCPolicyLabelValue>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0314E27C-272D-4EFB-AFDD-94BE43DF51E9}">
+  <dimension ref="B1:F104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="21"/>
+    <col min="3" max="3" width="10.140625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="16" style="21" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="21" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="68"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="31">
+        <v>1</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="69">
+        <v>0.9868055555555556</v>
+      </c>
+      <c r="F3" s="38">
+        <v>1446.64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="31">
+        <v>2</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="31">
+        <v>3</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="69">
+        <v>0.98888888888888893</v>
+      </c>
+      <c r="F5" s="38">
+        <v>1274.3800000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="31">
+        <v>4</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="69">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="F6" s="38">
+        <v>1700.1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="31">
+        <v>5</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="69">
+        <v>0.9902777777777777</v>
+      </c>
+      <c r="F7" s="38">
+        <v>2171.87</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="31">
+        <v>6</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="69">
+        <v>0.99097222222222225</v>
+      </c>
+      <c r="F8" s="38">
+        <v>1383.31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="31">
+        <v>7</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="69">
+        <v>0.9916666666666667</v>
+      </c>
+      <c r="F9" s="38">
+        <v>425.411</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="31">
+        <v>8</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="69">
+        <v>0.99236111111111114</v>
+      </c>
+      <c r="F10" s="38">
+        <v>1329.56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="31">
+        <v>9</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="69">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="F11" s="38">
+        <v>1462.02</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="31">
+        <v>10</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="69">
+        <v>0.99375000000000002</v>
+      </c>
+      <c r="F12" s="38">
+        <v>1301.94</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="31">
+        <v>11</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="69">
+        <v>0.99444444444444446</v>
+      </c>
+      <c r="F13" s="38">
+        <v>1333.59</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="31">
+        <v>12</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="69">
+        <v>0.99444444444444446</v>
+      </c>
+      <c r="F14" s="38">
+        <v>1634.38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="31">
+        <v>13</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="69">
+        <v>0.99513888888888891</v>
+      </c>
+      <c r="F15" s="38">
+        <v>1367.9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="31">
+        <v>14</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="69">
+        <v>0.99652777777777779</v>
+      </c>
+      <c r="F16" s="38">
+        <v>1582.96</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="31">
+        <v>15</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="69">
+        <v>0.99652777777777779</v>
+      </c>
+      <c r="F17" s="38">
+        <v>232.22300000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="31">
+        <v>16</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="69">
+        <v>0.99791666666666667</v>
+      </c>
+      <c r="F18" s="38">
+        <v>1725.1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="31">
+        <v>17</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="69">
+        <v>0.99791666666666667</v>
+      </c>
+      <c r="F19" s="38">
+        <v>1159.02</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="31">
+        <v>18</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="69">
+        <v>0.99861111111111101</v>
+      </c>
+      <c r="F20" s="38">
+        <v>1439.9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="31">
+        <v>19</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="69">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="F21" s="38">
+        <v>1278.45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="31">
+        <v>20</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="69">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F22" s="38">
+        <v>1482.93</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="31">
+        <v>21</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="69">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="F23" s="38">
+        <v>2704.79</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="31">
+        <v>22</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="69">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="F24" s="38">
+        <v>1224.02</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="31">
+        <v>23</v>
+      </c>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="38"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="31">
+        <v>24</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="69">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="F26" s="38">
+        <v>2362.75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="31">
+        <v>25</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="69">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="F27" s="38">
+        <v>1312.92</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="31">
+        <v>26</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="69">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="F28" s="38">
+        <v>1588.32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="31">
+        <v>27</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="69">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="F29" s="38">
+        <v>1176.8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="31">
+        <v>28</v>
+      </c>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="38"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="31">
+        <v>29</v>
+      </c>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="38"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="31">
+        <v>30</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="69">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="F32" s="38">
+        <v>2578.5300000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="31">
+        <v>31</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="69">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="F33" s="38">
+        <v>1613.73</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="31">
+        <v>32</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="69">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="F34" s="38">
+        <v>1137.2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="31">
+        <v>33</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" s="69">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="F35" s="38">
+        <v>406.83800000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="31">
+        <v>34</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="69">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F36" s="38">
+        <v>1002.55</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="31">
+        <v>35</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="69">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="F37" s="38">
+        <v>1184.5999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="31">
+        <v>36</v>
+      </c>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="38"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="31">
+        <v>37</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="69">
+        <v>1.2499999999999999E-2</v>
+      </c>
+      <c r="F39" s="38">
+        <v>1660.13</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="31">
+        <v>38</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="69">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="F40" s="38">
+        <v>3385.18</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="31">
+        <v>40</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="69">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="F41" s="38">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="31">
+        <v>41</v>
+      </c>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="38"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="31">
+        <v>42</v>
+      </c>
+      <c r="C43" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" s="69">
+        <v>1.5277777777777777E-2</v>
+      </c>
+      <c r="F43" s="38">
+        <v>3076.39</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="31">
+        <v>43</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" s="69">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="F44" s="38">
+        <v>2658.12</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="31">
+        <v>44</v>
+      </c>
+      <c r="C45" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E45" s="69">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F45" s="38">
+        <v>2271.42</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="31">
+        <v>45</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" s="69">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F46" s="38">
+        <v>1042.93</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="31">
+        <v>46</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E47" s="69">
+        <v>1.8055555555555557E-2</v>
+      </c>
+      <c r="F47" s="38">
+        <v>1186.75</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="31">
+        <v>47</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" s="69">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="F48" s="38">
+        <v>1546.48</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="31">
+        <v>48</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="69">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="F49" s="38">
+        <v>1415.33</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="31">
+        <v>49</v>
+      </c>
+      <c r="C50" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E50" s="69">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="F50" s="38">
+        <v>957.48800000000006</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="31">
+        <v>50</v>
+      </c>
+      <c r="C51" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" s="69">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="F51" s="38">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="31">
+        <v>51</v>
+      </c>
+      <c r="C52" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E52" s="69">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F52" s="38">
+        <v>1158.23</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="31">
+        <v>52</v>
+      </c>
+      <c r="C53" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E53" s="69">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="F53" s="38">
+        <v>2019.89</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="31">
+        <v>53</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D54" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E54" s="69">
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="F54" s="38">
+        <v>2603.5300000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="31">
+        <v>54</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55" s="69">
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="F55" s="38">
+        <v>2571.67</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="31">
+        <v>55</v>
+      </c>
+      <c r="C56" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D56" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E56" s="69">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="F56" s="38">
+        <v>2001.62</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="31">
+        <v>56</v>
+      </c>
+      <c r="C57" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" s="69">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F57" s="38">
+        <v>1743.34</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="31">
+        <v>57</v>
+      </c>
+      <c r="C58" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E58" s="69">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F58" s="38">
+        <v>1793.95</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="31">
+        <v>58</v>
+      </c>
+      <c r="C59" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E59" s="69">
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="F59" s="38">
+        <v>2049.79</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="31">
+        <v>59</v>
+      </c>
+      <c r="C60" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="69">
+        <v>2.7083333333333334E-2</v>
+      </c>
+      <c r="F60" s="38">
+        <v>1477.52</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="31">
+        <v>60</v>
+      </c>
+      <c r="C61" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E61" s="69">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="F61" s="38">
+        <v>6482.81</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="31">
+        <v>61</v>
+      </c>
+      <c r="C62" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="69">
+        <v>2.8472222222222222E-2</v>
+      </c>
+      <c r="F62" s="38">
+        <v>1823.7</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="31">
+        <v>62</v>
+      </c>
+      <c r="C63" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D63" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" s="69">
+        <v>2.9166666666666664E-2</v>
+      </c>
+      <c r="F63" s="38">
+        <v>1329.35</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="31">
+        <v>63</v>
+      </c>
+      <c r="C64" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D64" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E64" s="69">
+        <v>2.9861111111111113E-2</v>
+      </c>
+      <c r="F64" s="38">
+        <v>1452.32</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="31">
+        <v>64</v>
+      </c>
+      <c r="C65" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D65" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" s="69">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="F65" s="38">
+        <v>2788.96</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="31">
+        <v>65</v>
+      </c>
+      <c r="C66" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D66" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" s="69">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="F66" s="38">
+        <v>1909.88</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="31">
+        <v>66</v>
+      </c>
+      <c r="C67" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D67" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E67" s="69">
+        <v>3.1944444444444449E-2</v>
+      </c>
+      <c r="F67" s="38">
+        <v>2311.71</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="31">
+        <v>67</v>
+      </c>
+      <c r="C68" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E68" s="69">
+        <v>3.2638888888888891E-2</v>
+      </c>
+      <c r="F68" s="38">
+        <v>1073.04</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="31">
+        <v>68</v>
+      </c>
+      <c r="C69" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D69" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E69" s="69">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F69" s="38">
+        <v>2633.67</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="31">
+        <v>69</v>
+      </c>
+      <c r="C70" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D70" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E70" s="69">
+        <v>3.4027777777777775E-2</v>
+      </c>
+      <c r="F70" s="38">
+        <v>1655.03</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="31">
+        <v>70</v>
+      </c>
+      <c r="C71" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" s="69">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="F71" s="38">
+        <v>2733.89</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="31">
+        <v>71</v>
+      </c>
+      <c r="C72" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D72" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E72" s="69">
+        <v>3.5416666666666666E-2</v>
+      </c>
+      <c r="F72" s="38">
+        <v>1872.99</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="31">
+        <v>72</v>
+      </c>
+      <c r="C73" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E73" s="69">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="F73" s="38">
+        <v>2393.9699999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="31">
+        <v>73</v>
+      </c>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="38"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="31">
+        <v>74</v>
+      </c>
+      <c r="C75" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D75" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E75" s="69">
+        <v>3.6805555555555557E-2</v>
+      </c>
+      <c r="F75" s="38">
+        <v>934.75599999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="31">
+        <v>75</v>
+      </c>
+      <c r="C76" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D76" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E76" s="69">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="F76" s="38">
+        <v>1685.04</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="31">
+        <v>76</v>
+      </c>
+      <c r="C77" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D77" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E77" s="69">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="F77" s="38">
+        <v>1454.24</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="31">
+        <v>77</v>
+      </c>
+      <c r="C78" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D78" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E78" s="69">
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="F78" s="38">
+        <v>2001.13</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="31">
+        <v>78</v>
+      </c>
+      <c r="C79" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D79" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E79" s="69">
+        <v>4.027777777777778E-2</v>
+      </c>
+      <c r="F79" s="38">
+        <v>2288.11</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="31">
+        <v>79</v>
+      </c>
+      <c r="C80" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D80" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E80" s="69">
+        <v>4.027777777777778E-2</v>
+      </c>
+      <c r="F80" s="38">
+        <v>2301.0700000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="31">
+        <v>80</v>
+      </c>
+      <c r="C81" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D81" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E81" s="69">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F81" s="38">
+        <v>1210.33</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="31">
+        <v>81</v>
+      </c>
+      <c r="C82" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D82" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E82" s="69">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="F82" s="38">
+        <v>1271.8</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" s="31">
+        <v>82</v>
+      </c>
+      <c r="C83" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D83" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E83" s="69">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="F83" s="38">
+        <v>1386.81</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="31">
+        <v>83</v>
+      </c>
+      <c r="C84" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D84" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E84" s="69">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="F84" s="38">
+        <v>2077.25</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" s="31">
+        <v>84</v>
+      </c>
+      <c r="C85" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D85" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" s="69">
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="F85" s="38">
+        <v>1274.3800000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" s="31">
+        <v>85</v>
+      </c>
+      <c r="C86" s="37"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="38"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" s="31">
+        <v>86</v>
+      </c>
+      <c r="C87" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D87" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E87" s="69">
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="F87" s="38">
+        <v>2924.71</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B88" s="31">
+        <v>87</v>
+      </c>
+      <c r="C88" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D88" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E88" s="69">
+        <v>4.5833333333333337E-2</v>
+      </c>
+      <c r="F88" s="38">
+        <v>976.95</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" s="31">
+        <v>88</v>
+      </c>
+      <c r="C89" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D89" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E89" s="69">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="F89" s="38">
+        <v>2789.55</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B90" s="31">
+        <v>89</v>
+      </c>
+      <c r="C90" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D90" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E90" s="69">
+        <v>4.7916666666666663E-2</v>
+      </c>
+      <c r="F90" s="38">
+        <v>231.119</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" s="31">
+        <v>90</v>
+      </c>
+      <c r="C91" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D91" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E91" s="69">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="F91" s="38">
+        <v>3872.2</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" s="31">
+        <v>91</v>
+      </c>
+      <c r="C92" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D92" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E92" s="69">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="F92" s="38">
+        <v>2113.52</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" s="31">
+        <v>92</v>
+      </c>
+      <c r="C93" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D93" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E93" s="69">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="F93" s="38">
+        <v>1944.21</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94" s="31">
+        <v>93</v>
+      </c>
+      <c r="C94" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D94" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E94" s="69">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="F94" s="38">
+        <v>1357.15</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="31">
+        <v>94</v>
+      </c>
+      <c r="C95" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D95" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E95" s="69">
+        <v>5.1388888888888894E-2</v>
+      </c>
+      <c r="F95" s="38">
+        <v>2398.73</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B96" s="31">
+        <v>95</v>
+      </c>
+      <c r="C96" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D96" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E96" s="69">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="F96" s="38">
+        <v>2680.58</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B97" s="31">
+        <v>96</v>
+      </c>
+      <c r="C97" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D97" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E97" s="69">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="F97" s="38">
+        <v>1382.75</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B98" s="31">
+        <v>97</v>
+      </c>
+      <c r="C98" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D98" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E98" s="69">
+        <v>5.347222222222222E-2</v>
+      </c>
+      <c r="F98" s="38">
+        <v>1957.42</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B99" s="31">
+        <v>98</v>
+      </c>
+      <c r="C99" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D99" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E99" s="69">
+        <v>5.4166666666666669E-2</v>
+      </c>
+      <c r="F99" s="38">
+        <v>1313.27</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B100" s="31">
+        <v>99</v>
+      </c>
+      <c r="C100" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D100" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E100" s="69">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="F100" s="38">
+        <v>2213.14</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" s="31">
+        <v>100</v>
+      </c>
+      <c r="C101" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D101" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E101" s="69">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="F101" s="38">
+        <v>1691.13</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B102" s="31">
+        <v>101</v>
+      </c>
+      <c r="C102" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D102" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E102" s="69">
+        <v>5.6250000000000001E-2</v>
+      </c>
+      <c r="F102" s="38">
+        <v>3058.34</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B103" s="31">
+        <v>102</v>
+      </c>
+      <c r="C103" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D103" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E103" s="69">
+        <v>5.6944444444444443E-2</v>
+      </c>
+      <c r="F103" s="38">
+        <v>338.59399999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="70">
+        <v>103</v>
+      </c>
+      <c r="C104" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="D104" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="E104" s="72">
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="F104" s="73">
+        <v>2482.0700000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<p:Policy xmlns:p="office.server.policy" id="" local="true">
-  <p:Name>SurgicEye WordTemplate</p:Name>
-  <p:Description/>
-  <p:Statement/>
-  <p:PolicyItems>
-    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.Barcode" staticId="0x01010074A3F29CB79E8A41A92E73E19AE321CB00098C261D3F46DB49AEA371869FEC377C|-708099503" UniqueId="ce4bdff9-6a71-4ace-b157-8544c435bac6">
-      <p:Name>Barcodes</p:Name>
-      <p:Description>Generates unique identifiers that can be inserted in Microsoft Office documents. Barcodes can also be used to search for documents.</p:Description>
-      <p:CustomData>
-        <barcode/>
-      </p:CustomData>
-    </p:PolicyItem>
-    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.PolicyLabel" staticId="0x01010074A3F29CB79E8A41A92E73E19AE321CB00098C261D3F46DB49AEA371869FEC377C|801092262" UniqueId="22cbd58b-60ad-4bbd-a15c-010122a0c718">
-      <p:Name>Labels</p:Name>
-      <p:Description>Generates labels that can be inserted in Microsoft Office documents to ensure that document properties or other important information are included when documents are printed. Labels can also be used to search for documents.</p:Description>
-      <p:CustomData>
-        <label>
-          <segment type="metadata">_UIVersionString</segment>
-        </label>
-      </p:CustomData>
-    </p:PolicyItem>
-  </p:PolicyItems>
-</p:Policy>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="SurgicEye WordTemplate" ma:contentTypeID="0x01010074A3F29CB79E8A41A92E73E19AE321CB00098C261D3F46DB49AEA371869FEC377C" ma:contentTypeVersion="17" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="d27efd9bfa2cf0dc081f61d6777772ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e2656bbd-0e15-4aa0-af00-25744e385561" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53fececc5845ce19907e3af2573e5d2e" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9915,40 +11606,59 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAB86876-AAC8-4339-8E74-E0DFE2CA9AC3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="e2656bbd-0e15-4aa0-af00-25744e385561"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<p:Policy xmlns:p="office.server.policy" id="" local="true">
+  <p:Name>SurgicEye WordTemplate</p:Name>
+  <p:Description/>
+  <p:Statement/>
+  <p:PolicyItems>
+    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.Barcode" staticId="0x01010074A3F29CB79E8A41A92E73E19AE321CB00098C261D3F46DB49AEA371869FEC377C|-708099503" UniqueId="ce4bdff9-6a71-4ace-b157-8544c435bac6">
+      <p:Name>Barcodes</p:Name>
+      <p:Description>Generates unique identifiers that can be inserted in Microsoft Office documents. Barcodes can also be used to search for documents.</p:Description>
+      <p:CustomData>
+        <barcode/>
+      </p:CustomData>
+    </p:PolicyItem>
+    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.PolicyLabel" staticId="0x01010074A3F29CB79E8A41A92E73E19AE321CB00098C261D3F46DB49AEA371869FEC377C|801092262" UniqueId="22cbd58b-60ad-4bbd-a15c-010122a0c718">
+      <p:Name>Labels</p:Name>
+      <p:Description>Generates labels that can be inserted in Microsoft Office documents to ensure that document properties or other important information are included when documents are printed. Labels can also be used to search for documents.</p:Description>
+      <p:CustomData>
+        <label>
+          <segment type="metadata">_UIVersionString</segment>
+        </label>
+      </p:CustomData>
+    </p:PolicyItem>
+  </p:PolicyItems>
+</p:Policy>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3611D48C-6B4F-4CD9-8579-A2A41CE94ADA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A933A0-2E29-4D82-A4A8-6FECA8CC0598}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="office.server.policy"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DLCPolicyLabelClientValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">{_UIVersionString}</DLCPolicyLabelClientValue>
+    <_dlc_BarcodeImage xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">iVBORw0KGgoAAAANSUhEUgAAAYIAAABtCAYAAACsn2ZqAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAAAJcEhZcwAADsMAAA7DAcdvqGQAABp9SURBVHhe7ZvBihzbsiz3///0eeiBgeGE54qsTA0uSgMfWLt3aA2aqpH++9/Hx8fHxz/N90Xw8fHx8Y/zfRF8fHx8/ON8XwQfHx8f/zjfF8HHx8fHP873RfDx8fHxj/P6F8F///33/zORHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef3i1UOzwx3YdOBN6yZOW9yBk5u2deBpN+F97rbuQLppWwe27kxk533rwJs7nclu6w6km9MWd2DTTbStA80dSDfe5+5Xdyaya+5AumlbBzbd27x+8eqh2eEObDrwpnUTpy3uwMlN2zrwtJvwPndbdyDdtK0DW3cmsvO+deDNnc5kt3UH0s1pizuw6Sba1oHmDqQb73P3qzsT2TV3IN20rQOb7m1ev3j10OxwBzYdeNO6idMWd+Dkpm0deNpNeJ+7rTuQbtrWga07E9l53zrw5k5nstu6A+nmtMUd2HQTbetAcwfSjfe5+9WdieyaO5Bu2taBTfc2r1+8emh2uAObDrxp3cRpiztwctO2DjztJrzP3dYdSDdt68DWnYnsvG8deHOnM9lt3YF0c9riDmy6ibZ1oLkD6cb73P3qzkR2zR1IN23rwKZ7m9cvXj00O9yBTQfetG7itMUdOLlpWweedhPe527rDqSbtnVg685Edt63Dry505nstu5AujltcQc23UTbOtDcgXTjfe5+dWciu+YOpJu2dWDTvc3rF68emh3uwKYDb1o3cdriDpzctK0DT7sJ73O3dQfSTds6sHVnIjvvWwfe3OlMdlt3IN2ctrgDm26ibR1o7kC68T53v7ozkV1zB9JN2zqw6d7m9YtXD80Od2DTgTetmzhtcQdObtrWgafdhPe527oD6aZtHdi6M5Gd960Db+50JrutO5BuTlvcgU030bYONHcg3Xifu1/dmciuuQPppm0d2HRv8/rFq4dmhzuw6cCb1k2ctrgDJzdt68DTbsL73G3dgXTTtg5s3ZnIzvvWgTd3OpPd1h1IN6ct7sCmm2hbB5o7kG68z92v7kxk19yBdNO2Dmy6t3n94tVDs8Md2HTgTesmTlvcgZObtnXgaTfhfe627kC6aVsHtu5MZOd968CbO53JbusOpJvTFndg0020rQPNHUg33ufuV3cmsmvuQLppWwc23du8fvHqodnhDmw68KZ1E6ct7sDJTds68LSb8D53W3cg3bStA1t3JrLzvnXgzZ3OZLd1B9LNaYs7sOkm2taB5g6kG+9z96s7E9k1dyDdtK0Dm+5tXr949dDscAc2HXjTuonTFnfg5KZtHXjaTXifu607kG7a1oGtOxPZed868OZOZ7LbugPp5rTFHdh0E23rQHMH0o33ufvVnYnsmjuQbtrWgU33Nq9fvHpodrgDmw68ad3EaYs7cHLTtg487Sa8z93WHUg3bevA1p2J7LxvHXhzpzPZbd2BdHPa4g5suom2daC5A+nG+9z96s5Eds0dSDdt68Cme5vXL149NDvcgU0H3rRu4rTFHTi5aVsHnnYT3udu6w6km7Z1YOvORHbetw68udOZ7LbuQLo5bXEHNt1E2zrQ3IF0433ufnVnIrvmDqSbtnVg073N6xevHpod7sCmA29aN3Ha4g6c3LStA0+7Ce9zt3UH0k3bOrB1ZyI771sH3tzpTHZbdyDdnLa4A5tuom0daO5AuvE+d7+6M5FdcwfSTds6sOne5vWLVw/NDndg04E3rZs4bXEHTm7a1oGn3YT3udu6A+mmbR3YujORnfetA2/udCa7rTuQbk5b3IFNN9G2DjR3IN14n7tf3ZnIrrkD6aZtHdh0b/P6xauHZoc7sOnAm9ZNnLa4Ayc3bevA027C+9xt3YF007YObN2ZyM771oE3dzqT3dYdSDenLe7ApptoWweaO5BuvM/dr+5MZNfcgXTTtg5surd5/eLVQ7PDHdh04E3rJk5b3IGTm7Z14Gk34X3utu5AumlbB7buTGTnfevAmzudyW7rDqSb0xZ3YNNNtK0DzR1IN97n7ld3JrJr7kC6aVsHNt3bvH7x6qHZ4Q5sOvCmdROnLe7AyU3bOvC0m/A+d1t3IN20rQNbdyay87514M2dzmS3dQfSzWmLO7DpJtrWgeYOpBvvc/erOxPZNXcg3bStA5vubV6/ePXQ7HAHNh1407qJ0xZ34OSmbR142k14n7utO5Bu2taBrTsT2XnfOvDmTmey27oD6ea0xR3YdBNt60BzB9KN97n71Z2J7Jo7kG7a1oFN9zavX7x6aHa4A5sOvGndxGmLO3By07YOPO0mvM/d1h1IN23rwNadiey8bx14c6cz2W3dgXRz2uIObLqJtnWguQPpxvvc/erORHbNHUg3bevApnub1y9ePTQ73IFNB960buK0xR04uWlbB552E97nbusOpJu2dWDrzkR23rcOvLnTmey27kC6OW1xBzbdRNs60NyBdON97n51ZyK75g6km7Z1YNO9zesXrx6aHe7ApgNvWjdx2uIOnNy0rQNPuwnvc7d1B9JN2zqwdWciO+9bB97c6Ux2W3cg3Zy2uAObbqJtHWjuQLrxPne/ujORXXMH0k3bOrDp3ub1i1cPzQ53YNOBN62bOG1xB05u2taBp92E97nbugPppm0d2LozkZ33rQNv7nQmu607kG5OW9yBTTfRtg40dyDdeJ+7X92ZyK65A+mmbR3YdG/z+sWrh2aHO7DpwJvWTZy2uAMnN23rwNNuwvvcbd2BdNO2DmzdmcjO+9aBN3c6k93WHUg3py3uwKabaFsHmjuQbrzP3a/uTGTX3IF007YObLq3ef/ix8fHx8f/Kb4vgo+Pj49/nO+L4OPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+/irtP7/wH2OmwNQRc9XBWxu46k93snfMVffx8SbfX9fHX+XuB5j3m9+dNvmztzamdb/+W8nmzsfHW3x/WR9/hT8fWmRLbk+/e9XTbTZX5OaPk+Tqnrur3Yknv/vx0fj+qj7+Knc+uHJ7+t2rnm6zuaJtpp9v/63Nv9t48rsfH43vr+rjr7L94Jp2f36WSU4/m3q46v7wy+9OP8+f/fHMljvbj48t31/Vx19l+8H1ZPfnZ46Z9jB17U5yuru9A5vd9tbHx12+v6yPv8rf+IDzfvrd/FnbTD83V33r2r+14Zd/7+PjDb6/ro+/yuYD7O6HHPs7H5x/3OFnJ9pm+vnVvbf/rY+PN/n+wj7+KqcPsV8+5Pidq9/d3H2ymX7+N96z+b2Pj6d8f2Uff5XTB9kvH3T8ztXvvvXvtt308yfv+UNuNr/z8fEG31/ax1/lyYfj1G8+LN+4+4erO63b3Pl18/Hxt/j+2j7+Cn8+yDLJ9LPkdOMPp82ph80uN9Pu1P/htMne+fh4m++v6uPj4+Mf5/si+Pj4+PjH+b4IPj4+Pv5xvi+Cj4+Pj3+c74vg4+Pj4x/n+yL4+Pj4+Mf5vgg+Pj4+/nG+L4KPj4+Pf5r//e//AYQWEYJwHQKsAAAAAElFTkSuQmCC</_dlc_BarcodeImage>
+    <DLCPolicyLabelLock xmlns="e2656bbd-0e15-4aa0-af00-25744e385561" xsi:nil="true"/>
+    <_dlc_BarcodeValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">1758931852</_dlc_BarcodeValue>
+    <_dlc_BarcodePreview xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">
+      <Url>https://surgiceye.sharepoint.com/dev/_layouts/15/barcodeimagefromitem.aspx?ID=419111&amp;list=e2656bbd-0e15-4aa0-af00-25744e385561</Url>
+      <Description>Barcode: 1758931852</Description>
+    </_dlc_BarcodePreview>
+    <DLCPolicyLabelValue xmlns="e2656bbd-0e15-4aa0-af00-25744e385561">0.3</DLCPolicyLabelValue>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8953B42-7F0B-4652-8904-3F0A580F556B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9965,4 +11675,37 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A933A0-2E29-4D82-A4A8-6FECA8CC0598}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="office.server.policy"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3611D48C-6B4F-4CD9-8579-A2A41CE94ADA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAB86876-AAC8-4339-8E74-E0DFE2CA9AC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="e2656bbd-0e15-4aa0-af00-25744e385561"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>